<commit_message>
Work diary for the day
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="JdT-TPI_LRD" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -69,7 +69,22 @@
     <t>Le programme à crashé lors de la sauvegarde trois fois. Je refais la planification avec un autre programme</t>
   </si>
   <si>
-    <t>Sur GanttProject cette fois</t>
+    <t>9b11e557a8f607254b2b476a41fe98b5022022df</t>
+  </si>
+  <si>
+    <t>Remplissage de la sandbox sur Scrum</t>
+  </si>
+  <si>
+    <t>https://icescrum.cpnv.ch/p/NEWSWEBSIT/</t>
+  </si>
+  <si>
+    <t>Ajout du canvas de documentation</t>
+  </si>
+  <si>
+    <t>3b50924c0668f0b7c5f34f4eb16db6148d4fd43b</t>
+  </si>
+  <si>
+    <t>Sur GanttProject. Je ne suis pas 100% sûr du resultat. Elle sera révisée au besoin.</t>
   </si>
 </sst>
 </file>
@@ -406,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44683</v>
       </c>
@@ -531,14 +546,46 @@
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44683</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44683</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Documentation and work diary - PDF export
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="JdT-TPI_LRD" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,33 @@
   </si>
   <si>
     <t>Sur GanttProject. Je ne suis pas 100% sûr du resultat. Elle sera révisée au besoin.</t>
+  </si>
+  <si>
+    <t>Remplissage du fichier de documentation</t>
+  </si>
+  <si>
+    <t>Revue de la sandbox sur IceScrum avec CdP</t>
+  </si>
+  <si>
+    <t>Documentation de l'analyse concurentielle</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Définition de tests dans les story sur IceScrum</t>
+  </si>
+  <si>
+    <t>Préparation du premier rendu</t>
+  </si>
+  <si>
+    <t>39d1f2fc5b7a74535261ae7d8b8e759f4d303ebc</t>
+  </si>
+  <si>
+    <t>Remplissage du fichier de documentation - Cahier des charges et plus</t>
+  </si>
+  <si>
+    <t>J'ai oublié de faire le rendu de la planification initiale le premier soir</t>
   </si>
 </sst>
 </file>
@@ -421,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +488,9 @@
       <c r="A2" s="2">
         <v>44683</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
@@ -472,6 +502,9 @@
       <c r="A3" s="2">
         <v>44683</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C3" s="1">
         <v>0.25</v>
       </c>
@@ -489,6 +522,9 @@
       <c r="A4" s="2">
         <v>44683</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C4" s="1">
         <v>0.25</v>
       </c>
@@ -500,6 +536,9 @@
       <c r="A5" s="2">
         <v>44683</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C5" s="1">
         <v>0.25</v>
       </c>
@@ -514,6 +553,9 @@
       <c r="A6" s="2">
         <v>44683</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C6" s="1">
         <v>0.25</v>
       </c>
@@ -525,6 +567,9 @@
       <c r="A7" s="2">
         <v>44683</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C7" s="1">
         <v>2.25</v>
       </c>
@@ -539,6 +584,9 @@
       <c r="A8" s="2">
         <v>44683</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C8" s="1">
         <v>1.5</v>
       </c>
@@ -556,6 +604,9 @@
       <c r="A9" s="2">
         <v>44683</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C9" s="1">
         <v>0.75</v>
       </c>
@@ -566,9 +617,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44683</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -578,14 +632,129 @@
       </c>
       <c r="F10" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>44684</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>44684</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>44684</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44684</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>44684</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>44684</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>44684</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="E9" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId4"/>
+  <headerFooter>
+    <oddHeader>&amp;LCPNV</oddHeader>
+    <oddFooter>&amp;LLouis Richard - louis.richard@cpnv.ch&amp;C&amp;P/&amp;N&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
documentation and today's work diary
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="JdT-TPI_LRD" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -112,6 +112,51 @@
   </si>
   <si>
     <t>J'ai oublié de faire le rendu de la planification initiale le premier soir</t>
+  </si>
+  <si>
+    <t>Model Conceptuel de Donée (MCD)</t>
+  </si>
+  <si>
+    <t>9edae5173994be5b0d1cb6a1197305bcb657c620</t>
+  </si>
+  <si>
+    <t>Revue de la documentation, de la planification et du MCD avec chef de projet</t>
+  </si>
+  <si>
+    <t>Révision du MCD, problème du stockage des images. Modification de la planification détaillée dans le point Historique de la documentation</t>
+  </si>
+  <si>
+    <t>07cf448ff6cb71c152bda1016a0b338bfc1fb162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation : Introduction et stratégie de test </t>
+  </si>
+  <si>
+    <t>Modification de la planification initiale : répartition de l'analyse dans chaque sprint plus adapté à la méthode agile et repartissions de la charge de travail</t>
+  </si>
+  <si>
+    <t>Définition de tâches sur IceScrum</t>
+  </si>
+  <si>
+    <t>Documentation : Introduction, historique et développement du budget</t>
+  </si>
+  <si>
+    <t>Conception</t>
+  </si>
+  <si>
+    <t>Premier design du MLD</t>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <t>Aide à camarade Bryan Evangelisti</t>
+  </si>
+  <si>
+    <t>d4483afbe21c49cfcf5071c56c0fc4bc242e1f7a</t>
+  </si>
+  <si>
+    <t>Définition des objectifs</t>
   </si>
 </sst>
 </file>
@@ -172,7 +217,33 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -183,6 +254,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F26" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:F26"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Date" dataDxfId="7"/>
+    <tableColumn id="2" name="Type" dataDxfId="6"/>
+    <tableColumn id="3" name="Durée (heures)" dataDxfId="5"/>
+    <tableColumn id="4" name="Description" dataDxfId="4"/>
+    <tableColumn id="5" name="Remarque" dataDxfId="3"/>
+    <tableColumn id="6" name="Commit ID" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,23 +534,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="66.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44683</v>
       </c>
@@ -498,7 +584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44683</v>
       </c>
@@ -518,7 +604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44683</v>
       </c>
@@ -532,7 +618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44683</v>
       </c>
@@ -549,7 +635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44683</v>
       </c>
@@ -563,7 +649,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44683</v>
       </c>
@@ -579,8 +665,12 @@
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f>SUM(C:C)</f>
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44683</v>
       </c>
@@ -600,7 +690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44683</v>
       </c>
@@ -617,7 +707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44683</v>
       </c>
@@ -634,7 +724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44684</v>
       </c>
@@ -648,7 +738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44684</v>
       </c>
@@ -665,7 +755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44684</v>
       </c>
@@ -682,7 +772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44684</v>
       </c>
@@ -695,8 +785,11 @@
       <c r="D14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44684</v>
       </c>
@@ -713,7 +806,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44684</v>
       </c>
@@ -727,7 +820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44684</v>
       </c>
@@ -742,6 +835,135 @@
       </c>
       <c r="E17" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>44686</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>44686</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>44686</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>44686</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44686</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44686</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>44686</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>44686</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>44687</v>
       </c>
     </row>
   </sheetData>
@@ -756,5 +978,8 @@
     <oddHeader>&amp;LCPNV</oddHeader>
     <oddFooter>&amp;LLouis Richard - louis.richard@cpnv.ch&amp;C&amp;P/&amp;N&amp;R&amp;D</oddFooter>
   </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Documentation and work diary
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -190,6 +190,33 @@
   </si>
   <si>
     <t>6369b468d2611907f95278f0fdac075f4a37b030</t>
+  </si>
+  <si>
+    <t>Révision du MCD</t>
+  </si>
+  <si>
+    <t>b7a8224aafc0a5275e8de50b1984fc9afd59a5ce</t>
+  </si>
+  <si>
+    <t>Comme suggérer dans un email du chef de projet</t>
+  </si>
+  <si>
+    <t>Estimation des story et activation du sprint</t>
+  </si>
+  <si>
+    <t>Selon MCD</t>
+  </si>
+  <si>
+    <t>ab90804b5cba1e50fe3f048a65b95861cc596981</t>
+  </si>
+  <si>
+    <t>Définition de la stratégie de test pour nouvelles stories</t>
+  </si>
+  <si>
+    <t>Modification de la documentation</t>
+  </si>
+  <si>
+    <t>Utilisation des nouveaux MCD et MLD</t>
   </si>
 </sst>
 </file>
@@ -290,8 +317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F35" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F35"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -567,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +607,7 @@
     <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="66.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -700,7 +727,7 @@
       </c>
       <c r="H7">
         <f>SUM(C:C)</f>
-        <v>23.5</v>
+        <v>25.75</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1077,6 +1104,91 @@
       </c>
       <c r="E30" s="1" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>44690</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>44690</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44690</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>44690</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>44690</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work diary of the latest bugfix
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF1741F-757E-49A7-BA7A-41A268E86B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JdT-TPI_LRD" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -259,12 +270,21 @@
   </si>
   <si>
     <t>Documentation du projet</t>
+  </si>
+  <si>
+    <t>BugFix du bug d'hier</t>
+  </si>
+  <si>
+    <t>prepare : mauvaise définiton des return dans la documentation de la fonction. Fonction non-définie : &lt;?php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -312,6 +332,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -336,7 +359,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -359,15 +382,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:F44" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Date" dataDxfId="5"/>
-    <tableColumn id="2" name="Type" dataDxfId="4"/>
-    <tableColumn id="3" name="Durée (heures)" dataDxfId="3"/>
-    <tableColumn id="4" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" name="Remarque" dataDxfId="1"/>
-    <tableColumn id="6" name="Commit ID" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Durée (heures)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Remarque" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Commit ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -635,16 +658,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="66.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -769,7 +792,7 @@
       </c>
       <c r="H7">
         <f>SUM(C:C)</f>
-        <v>33.75</v>
+        <v>36.25</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1363,11 +1386,28 @@
         <v>79</v>
       </c>
     </row>
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>44692</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E9" r:id="rId2"/>
-    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
Work diary for the morning
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF1741F-757E-49A7-BA7A-41A268E86B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="JdT-TPI_LRD" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -276,15 +275,15 @@
   </si>
   <si>
     <t>prepare : mauvaise définiton des return dans la documentation de la fonction. Fonction non-définie : &lt;?php</t>
+  </si>
+  <si>
+    <t>Vérification de l'email de l'utilisateur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -334,7 +333,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -359,7 +358,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -382,15 +381,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:F44" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F45"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Durée (heures)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Remarque" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Commit ID" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" name="Type" dataDxfId="4"/>
+    <tableColumn id="3" name="Durée (heures)" dataDxfId="3"/>
+    <tableColumn id="4" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" name="Remarque" dataDxfId="1"/>
+    <tableColumn id="6" name="Commit ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,11 +657,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +791,7 @@
       </c>
       <c r="H7">
         <f>SUM(C:C)</f>
-        <v>36.25</v>
+        <v>39.25</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1403,11 +1402,25 @@
         <v>81</v>
       </c>
     </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>44693</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
Work diary so far
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -281,6 +281,12 @@
   </si>
   <si>
     <t>7abc0e45b4b63950fc36fa59d6ca8f9b21ca75bb</t>
+  </si>
+  <si>
+    <t>réalisation</t>
+  </si>
+  <si>
+    <t>Paufinage de la vérification de l'email, activation de l'utilisateur, email tout bien</t>
   </si>
 </sst>
 </file>
@@ -384,8 +390,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F46" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F46"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -661,7 +667,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
@@ -794,7 +800,7 @@
       </c>
       <c r="H7">
         <f>SUM(C:C)</f>
-        <v>39.25</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1420,6 +1426,20 @@
       </c>
       <c r="F45" s="1" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>44693</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work diary for yesterday and today so far
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>Paufinage de la vérification de l'email, activation de l'utilisateur, email tout bien</t>
+  </si>
+  <si>
+    <t>Commencement de la fonction de login</t>
+  </si>
+  <si>
+    <t>Finition de la fonction de login</t>
   </si>
 </sst>
 </file>
@@ -390,8 +396,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F46" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F48" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F48"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -667,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +806,7 @@
       </c>
       <c r="H7">
         <f>SUM(C:C)</f>
-        <v>41.5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1440,6 +1446,34 @@
       </c>
       <c r="D46" s="1" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>44693</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>44694</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work diary for the last 45 minutes
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -299,6 +299,15 @@
   </si>
   <si>
     <t>c25f4ed08a8cc4a94f4295f148e7d4cfb7c2b781</t>
+  </si>
+  <si>
+    <t>Gestions des erreurs/exceptions</t>
+  </si>
+  <si>
+    <t>Affichage du message d'erreur a l'utilisateur</t>
+  </si>
+  <si>
+    <t>76e90026b3f5ee849f3a2f6bb866614cdf21086e</t>
   </si>
 </sst>
 </file>
@@ -343,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -355,6 +364,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -402,8 +414,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F48" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F49" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F49"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -679,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +824,7 @@
       </c>
       <c r="H7">
         <f>SUM(C:C)</f>
-        <v>43</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1486,6 +1498,26 @@
       </c>
       <c r="F48" s="1" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>44694</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work diary for this morning
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>76e90026b3f5ee849f3a2f6bb866614cdf21086e</t>
+  </si>
+  <si>
+    <t>Correction des bugs présents afin de passer les tests d'acceptations</t>
   </si>
 </sst>
 </file>
@@ -414,8 +417,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F49" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F50" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F50"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -691,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +827,7 @@
       </c>
       <c r="H7">
         <f>SUM(C:C)</f>
-        <v>43.75</v>
+        <v>44.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1518,6 +1521,20 @@
       </c>
       <c r="F49" s="5" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>44694</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review with product owner
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Correction des bugs présents afin de passer les tests d'acceptations</t>
+  </si>
+  <si>
+    <t>Quelques trucs a réviser. Voir dans documentation/review</t>
   </si>
 </sst>
 </file>
@@ -417,8 +420,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F50" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F51" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F51"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -694,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,7 +830,7 @@
       </c>
       <c r="H7">
         <f>SUM(C:C)</f>
-        <v>44.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1535,6 +1538,23 @@
       </c>
       <c r="D50" s="1" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>44694</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week done. Documentation and work diary
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -314,6 +314,15 @@
   </si>
   <si>
     <t>Quelques trucs a réviser. Voir dans documentation/review</t>
+  </si>
+  <si>
+    <t>Revue des commentaires, définitions de fonctions, etc</t>
+  </si>
+  <si>
+    <t>Reprise de la documentation du projet</t>
+  </si>
+  <si>
+    <t>Pas beaucoup de documentation cette semaine</t>
   </si>
 </sst>
 </file>
@@ -420,8 +429,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F51" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F53" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F53"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -697,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +722,7 @@
     <col min="6" max="6" width="43.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44683</v>
       </c>
@@ -747,7 +756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44683</v>
       </c>
@@ -767,7 +776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44683</v>
       </c>
@@ -781,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44683</v>
       </c>
@@ -798,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44683</v>
       </c>
@@ -812,7 +821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44683</v>
       </c>
@@ -828,12 +837,8 @@
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H7">
-        <f>SUM(C:C)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44683</v>
       </c>
@@ -853,7 +858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44683</v>
       </c>
@@ -870,7 +875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44683</v>
       </c>
@@ -887,7 +892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44684</v>
       </c>
@@ -901,7 +906,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44684</v>
       </c>
@@ -918,7 +923,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44684</v>
       </c>
@@ -935,7 +940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44684</v>
       </c>
@@ -952,7 +957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44684</v>
       </c>
@@ -969,7 +974,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44684</v>
       </c>
@@ -1555,6 +1560,37 @@
       </c>
       <c r="E51" s="1" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>44694</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>44694</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work diary so I don't forget
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="120">
   <si>
     <t>Date</t>
   </si>
@@ -373,6 +373,12 @@
   </si>
   <si>
     <t>Protection contre injections SQL dans l'ajout d'article et gestion d'Exceptions</t>
+  </si>
+  <si>
+    <t>Création de la page d'affichage pour un article</t>
+  </si>
+  <si>
+    <t>Accessible (pour le moment) que depuis le carousel de la home page</t>
   </si>
 </sst>
 </file>
@@ -759,7 +765,7 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,9 +1819,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>44700</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work diary and documentation so far
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="128">
   <si>
     <t>Date</t>
   </si>
@@ -382,6 +382,27 @@
   </si>
   <si>
     <t xml:space="preserve">Affichage des articles sur la page d'acceuil </t>
+  </si>
+  <si>
+    <t>Correction de quelques bugs et préparation de la visite du second expert</t>
+  </si>
+  <si>
+    <t>Visite</t>
+  </si>
+  <si>
+    <t>Visite du second expert</t>
+  </si>
+  <si>
+    <t>Définition des tests effectués et écriture de plus de tests</t>
+  </si>
+  <si>
+    <t>Journal de travail pas assez précis. Bien faire attention a tout noter. Documentation en retard. Partie réalisation pas encore entamée. En retard sur le code. Il ne reste que 4 jours de travail pour implémenter les fonctionnalités manquantes et mettre le site en ligne. L'expert se montre inquiet</t>
+  </si>
+  <si>
+    <t>Pareil que la visite de l'expert.</t>
+  </si>
+  <si>
+    <t>Bugfix - Tests de la story "ajout d'articles"</t>
   </si>
 </sst>
 </file>
@@ -488,8 +509,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F65" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F70" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F70"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -765,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,7 +1860,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>44700</v>
       </c>
@@ -1851,6 +1872,79 @@
       </c>
       <c r="D65" s="1" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>44701</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>44701</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>44701</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>44701</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>44701</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work diary and documentation
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1A383F-96AC-4683-91F9-D4BAE65182E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JdT-TPI_LRD" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="129">
   <si>
     <t>Date</t>
   </si>
@@ -403,12 +404,18 @@
   </si>
   <si>
     <t>Bugfix - Tests de la story "ajout d'articles"</t>
+  </si>
+  <si>
+    <t>Fonction de like et dislike</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -462,6 +469,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -486,7 +496,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -509,15 +519,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F70" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:F71" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F71" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Date" dataDxfId="5"/>
-    <tableColumn id="2" name="Type" dataDxfId="4"/>
-    <tableColumn id="3" name="Durée (heures)" dataDxfId="3"/>
-    <tableColumn id="4" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" name="Remarque" dataDxfId="1"/>
-    <tableColumn id="6" name="Commit ID" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Durée (heures)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Remarque" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Commit ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -785,11 +795,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,15 +1953,32 @@
       <c r="B70" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
       <c r="D70" s="1" t="s">
         <v>127</v>
       </c>
     </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>44703</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E9" r:id="rId2"/>
-    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
Documentation of the Like/dislike function
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="131">
   <si>
     <t>Date</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>Documentation des tests effectués</t>
+  </si>
+  <si>
+    <t>Fonction like/dislike</t>
+  </si>
+  <si>
+    <t>Documentation de la fonction like/dislike</t>
   </si>
 </sst>
 </file>
@@ -512,8 +518,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F71" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F73" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F73"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -789,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,6 +1971,34 @@
       </c>
       <c r="D71" s="1" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>44703</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>44704</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mockups of author and category manager
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="137">
   <si>
     <t>Date</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>Documentation de la nouvelle feature</t>
+  </si>
+  <si>
+    <t>Maquettes des fonctionnalités a venir</t>
   </si>
 </sst>
 </file>
@@ -533,8 +536,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F77" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F78" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F78"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -810,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2073,6 +2076,20 @@
       </c>
       <c r="D77" s="1" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>44704</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add and delete authors
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
   <si>
     <t>Date</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>Page de gestion des auteurs et ajout d'un auteur</t>
+  </si>
+  <si>
+    <t>Suppression d'auteur</t>
   </si>
 </sst>
 </file>
@@ -539,8 +542,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F79" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F81" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F81"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -816,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,6 +2110,34 @@
       </c>
       <c r="D79" s="1" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>44704</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>44704</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work diary - comments
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="140">
   <si>
     <t>Date</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>Suppression d'auteur</t>
+  </si>
+  <si>
+    <t>Revue des commentaires</t>
   </si>
 </sst>
 </file>
@@ -542,8 +545,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F81" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F82" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -819,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,6 +2141,20 @@
       </c>
       <c r="D81" s="1" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>44704</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documentation of the comment function
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="145">
   <si>
     <t>Date</t>
   </si>
@@ -445,6 +445,15 @@
   </si>
   <si>
     <t>Préparation du serveur distant pour le site</t>
+  </si>
+  <si>
+    <t>Tentative d'ajout de commentaires</t>
+  </si>
+  <si>
+    <t>Ne fonctionne pas du à une erreur FK SQL</t>
+  </si>
+  <si>
+    <t>Documentation des tests des commentaires</t>
   </si>
 </sst>
 </file>
@@ -551,8 +560,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F84" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F87" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F87"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -828,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,7 +2144,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>44704</v>
       </c>
@@ -2149,7 +2158,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>44704</v>
       </c>
@@ -2163,7 +2172,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>44704</v>
       </c>
@@ -2177,7 +2186,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>44704</v>
       </c>
@@ -2190,6 +2199,40 @@
       <c r="D84" s="1" t="s">
         <v>141</v>
       </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>44705</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>44705</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C86" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Modified doc to fit new features
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -454,6 +454,15 @@
   </si>
   <si>
     <t>Documentation des tests des commentaires</t>
+  </si>
+  <si>
+    <t>Visite chef de projet -&gt; Deboggage de l'ajout de commentaires</t>
+  </si>
+  <si>
+    <t>Récupération des commentaires pour un article</t>
+  </si>
+  <si>
+    <t>Édition de la doc selon modifications requises pour l'ajout de commentaires</t>
   </si>
 </sst>
 </file>
@@ -560,8 +569,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F87" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F87"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F89" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F89"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Type" dataDxfId="4"/>
@@ -837,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,7 +2241,46 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
+      <c r="A87" s="4">
+        <v>44705</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C87" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>44705</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>44705</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>